<commit_message>
Add SQL scripts, update credit card project, remove Advanced
Added new SQL scripts for JOIN operations and date/time functions in Beginner/Script. Updated the Credit Card project with a new database file, expanded table creation script, and updated dataset. Updated lecture slides for Lec_5_6 and Lec_9_10. Removed the obsolete 'Advanced' file.
</commit_message>
<xml_diff>
--- a/Beginner/Project/Credit Card/Dataset_Credit_Card.xlsx
+++ b/Beginner/Project/Credit Card/Dataset_Credit_Card.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10720"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10727"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xiaotingzhou/Documents/Lectures/SQL/Beginner/Project/Credit Card/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57E61D3B-D23B-8142-A2F8-207CE7148DA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB9334C3-4CC2-A247-88B1-7354D3111B18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="18380" activeTab="4" xr2:uid="{4F4E6C32-125B-FC44-9721-F24B365705FA}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="29400" windowHeight="18360" activeTab="4" xr2:uid="{4F4E6C32-125B-FC44-9721-F24B365705FA}"/>
   </bookViews>
   <sheets>
     <sheet name="fraudTrain" sheetId="1" r:id="rId1"/>
@@ -4573,7 +4573,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="4" topLeftCell="E1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E18" sqref="E18"/>
+      <selection pane="topRight" activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="25.1640625" defaultRowHeight="19"/>
@@ -8444,7 +8444,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDDD8D6C-F126-8540-A3C2-1B86E44E74E1}">
   <dimension ref="A1:D53"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="C3" zoomScale="117" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="90" workbookViewId="0">
       <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
@@ -8802,9 +8802,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33547C99-7D60-EC4E-8B16-E9FF6C0FB7E4}">
   <dimension ref="A1:D147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="81" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="23"/>
   <cols>

</xml_diff>